<commit_message>
Number of matches by school.
</commit_message>
<xml_diff>
--- a/YouScienceData/Career Fairs Planning.xlsx
+++ b/YouScienceData/Career Fairs Planning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Desktop/YouScience/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/YouScienceData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7DC152-EAF0-0644-935A-C854AE5F38D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B90141-0A31-0B4D-B9F1-298116A49D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22500" windowHeight="20200" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22500" windowHeight="20100" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackman MS_Blackman HS" sheetId="1" r:id="rId1"/>
@@ -3186,8 +3186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3706,8 +3706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A208E7-51F2-4750-971F-40A4581FD6A3}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4176,7 +4176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CA9B03-A8CF-40DC-B290-BC4059AC973A}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -4700,8 +4700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CAF890-513F-44D2-B750-4E1C6BB30415}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4825,8 +4825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE52430B-BFEF-4BEF-AD3F-1299133F8B88}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5296,7 +5296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB24497C-1EBC-4F58-B27E-D2242AA49D48}">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -5846,8 +5846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91486225-7CD7-4453-82DE-FE7D204837CC}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6380,8 +6380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CE2F78-A302-4A9E-9C0C-2D8C8F9CB714}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6954,8 +6954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDB4EC6-1FD4-41F3-A1BA-FFBC4283C54D}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7073,8 +7073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA5B74F-6151-4DC9-AEF7-64A54C84A6B8}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7144,7 +7144,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B6" t="s">
@@ -7188,8 +7188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B01AC3-4DCB-4402-809B-04F49CAE1071}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7590,8 +7590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831DB09C-68EA-43E0-8EAD-F417EAA97127}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8250,8 +8250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B96BAC8-7A72-477D-A246-A02F0412314F}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8826,8 +8826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0ECAA3E-5F0F-44BF-B150-4C1247FE1FB1}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9321,8 +9321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94161DD7-51E3-49DA-813F-D163D6F61167}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9853,5 +9853,6 @@
     <hyperlink ref="G10" r:id="rId38" xr:uid="{2153A4EA-B5CA-459B-BD00-F83587451269}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>